<commit_message>
Ready for first trials
</commit_message>
<xml_diff>
--- a/Data/Annotations_124839_primers.xlsx
+++ b/Data/Annotations_124839_primers.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0099120\Dropbox\Shared R projects\RT-qPCR\RT-qPCR\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\u0099120\Dropbox\Shared R projects\qpcrviia7\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6510" yWindow="0" windowWidth="18540" windowHeight="11895"/>
+    <workbookView xWindow="7440" yWindow="0" windowWidth="18540" windowHeight="11895"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="37">
   <si>
     <t>Target 1</t>
   </si>
@@ -125,10 +125,16 @@
     <t>Gene</t>
   </si>
   <si>
-    <t>Primer</t>
-  </si>
-  <si>
     <t>HKG</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Target</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
   <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -461,13 +467,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
         <v>32</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>33</v>
-      </c>
-      <c r="C1" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -477,8 +483,8 @@
       <c r="B2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="b">
-        <v>1</v>
+      <c r="C2" t="s">
+        <v>34</v>
       </c>
       <c r="D2" s="1"/>
     </row>
@@ -489,8 +495,8 @@
       <c r="B3" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="b">
-        <v>1</v>
+      <c r="C3" t="s">
+        <v>34</v>
       </c>
       <c r="D3" s="1"/>
     </row>
@@ -501,8 +507,8 @@
       <c r="B4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="b">
-        <v>1</v>
+      <c r="C4" t="s">
+        <v>34</v>
       </c>
       <c r="D4" s="1"/>
     </row>
@@ -513,8 +519,8 @@
       <c r="B5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="b">
-        <v>0</v>
+      <c r="C5" t="s">
+        <v>35</v>
       </c>
       <c r="D5" s="1"/>
     </row>
@@ -525,8 +531,8 @@
       <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="b">
-        <v>0</v>
+      <c r="C6" t="s">
+        <v>35</v>
       </c>
       <c r="D6" s="1"/>
     </row>
@@ -537,8 +543,8 @@
       <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="C7" t="b">
-        <v>0</v>
+      <c r="C7" t="s">
+        <v>35</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -549,8 +555,8 @@
       <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="C8" t="b">
-        <v>0</v>
+      <c r="C8" t="s">
+        <v>35</v>
       </c>
       <c r="D8" s="1"/>
     </row>
@@ -561,8 +567,8 @@
       <c r="B9" t="s">
         <v>22</v>
       </c>
-      <c r="C9" t="b">
-        <v>0</v>
+      <c r="C9" t="s">
+        <v>35</v>
       </c>
       <c r="D9" s="1"/>
     </row>
@@ -573,8 +579,8 @@
       <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" t="b">
-        <v>0</v>
+      <c r="C10" t="s">
+        <v>35</v>
       </c>
       <c r="D10" s="1"/>
     </row>
@@ -585,8 +591,8 @@
       <c r="B11" t="s">
         <v>23</v>
       </c>
-      <c r="C11" t="b">
-        <v>0</v>
+      <c r="C11" t="s">
+        <v>35</v>
       </c>
       <c r="D11" s="1"/>
     </row>
@@ -597,8 +603,8 @@
       <c r="B12" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="b">
-        <v>0</v>
+      <c r="C12" t="s">
+        <v>35</v>
       </c>
       <c r="D12" s="1"/>
     </row>
@@ -609,8 +615,8 @@
       <c r="B13" t="s">
         <v>26</v>
       </c>
-      <c r="C13" t="b">
-        <v>0</v>
+      <c r="C13" t="s">
+        <v>35</v>
       </c>
       <c r="D13" s="1"/>
     </row>
@@ -621,8 +627,8 @@
       <c r="B14" t="s">
         <v>27</v>
       </c>
-      <c r="C14" t="b">
-        <v>0</v>
+      <c r="C14" t="s">
+        <v>35</v>
       </c>
       <c r="D14" s="1"/>
     </row>
@@ -633,8 +639,8 @@
       <c r="B15" t="s">
         <v>28</v>
       </c>
-      <c r="C15" t="b">
-        <v>0</v>
+      <c r="C15" t="s">
+        <v>35</v>
       </c>
       <c r="D15" s="1"/>
     </row>
@@ -645,8 +651,8 @@
       <c r="B16" t="s">
         <v>29</v>
       </c>
-      <c r="C16" t="b">
-        <v>0</v>
+      <c r="C16" t="s">
+        <v>35</v>
       </c>
       <c r="D16" s="1"/>
     </row>
@@ -657,8 +663,8 @@
       <c r="B17" t="s">
         <v>30</v>
       </c>
-      <c r="C17" t="b">
-        <v>0</v>
+      <c r="C17" t="s">
+        <v>35</v>
       </c>
       <c r="D17" s="1"/>
     </row>

</xml_diff>